<commit_message>
adding new excel spreadsheet
</commit_message>
<xml_diff>
--- a/Clue_Board_Layout_Langfield_Prather.xlsx
+++ b/Clue_Board_Layout_Langfield_Prather.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlangfield/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexlangfield/Desktop/Software_Engineering/Clue-Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="32">
   <si>
     <t>L</t>
   </si>
@@ -87,13 +87,52 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>X, Testing for edge</t>
+  </si>
+  <si>
+    <t>Y, test</t>
+  </si>
+  <si>
+    <t>O, test</t>
+  </si>
+  <si>
+    <t>AdjWallTest</t>
+  </si>
+  <si>
+    <t>RoomAdjecenct</t>
+  </si>
+  <si>
+    <t>CantGoOffBoard</t>
+  </si>
+  <si>
+    <t>DoorWayCheck</t>
+  </si>
+  <si>
+    <t>CanGoIntoDoorway</t>
+  </si>
+  <si>
+    <t>OnlyGoInDoor</t>
+  </si>
+  <si>
+    <t>Can'tGoThroughWalls</t>
+  </si>
+  <si>
+    <t>GoingIntoRoom with targets</t>
+  </si>
+  <si>
+    <t>LeavingARoom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,8 +140,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +195,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -184,10 +321,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -196,10 +334,44 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="64" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,8 +683,8 @@
       <c r="I1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>5</v>
+      <c r="J1" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>5</v>
@@ -721,7 +893,7 @@
       <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="26" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -733,19 +905,19 @@
       <c r="I4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="26" t="s">
         <v>19</v>
       </c>
       <c r="O4" s="5" t="s">
@@ -795,7 +967,7 @@
       <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -810,10 +982,10 @@
       <c r="J5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="34" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -846,7 +1018,7 @@
       <c r="V5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="W5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="X5">
@@ -887,13 +1059,13 @@
       <c r="K6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="28" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="17" t="s">
         <v>19</v>
       </c>
       <c r="O6" s="5" t="s">
@@ -911,7 +1083,7 @@
       <c r="S6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="5" t="s">
+      <c r="T6" s="19" t="s">
         <v>13</v>
       </c>
       <c r="U6" s="5" t="s">
@@ -988,13 +1160,13 @@
       <c r="T7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="19" t="s">
         <v>13</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="W7" s="2" t="s">
+      <c r="W7" s="12" t="s">
         <v>19</v>
       </c>
       <c r="X7">
@@ -1011,7 +1183,7 @@
       <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="19" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1050,7 +1222,7 @@
       <c r="P8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="19" t="s">
         <v>14</v>
       </c>
       <c r="R8" s="5" t="s">
@@ -1059,7 +1231,7 @@
       <c r="S8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="T8" s="30" t="s">
         <v>19</v>
       </c>
       <c r="U8" s="2" t="s">
@@ -1082,13 +1254,13 @@
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="33" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -1097,37 +1269,37 @@
       <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="9" t="s">
+      <c r="H9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="P9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="R9" s="19" t="s">
         <v>14</v>
       </c>
       <c r="S9" s="2" t="s">
@@ -1159,7 +1331,7 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="12" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1171,25 +1343,25 @@
       <c r="G10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="9" t="s">
+      <c r="H10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O10" s="2" t="s">
@@ -1198,7 +1370,7 @@
       <c r="P10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="2" t="s">
+      <c r="Q10" s="33" t="s">
         <v>19</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -1207,7 +1379,7 @@
       <c r="S10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="2" t="s">
+      <c r="T10" s="17" t="s">
         <v>19</v>
       </c>
       <c r="U10" s="2" t="s">
@@ -1245,25 +1417,25 @@
       <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="9" t="s">
+      <c r="H11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O11" s="2" t="s">
@@ -1319,25 +1491,25 @@
       <c r="G12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="9" t="s">
+      <c r="H12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O12" s="2" t="s">
@@ -1352,7 +1524,7 @@
       <c r="R12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="28" t="s">
         <v>19</v>
       </c>
       <c r="T12" s="2" t="s">
@@ -1393,25 +1565,25 @@
       <c r="G13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="9" t="s">
+      <c r="H13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O13" s="2" t="s">
@@ -1423,22 +1595,22 @@
       <c r="Q13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="R13" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="U13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W13" s="5" t="s">
+      <c r="T13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="19" t="s">
         <v>4</v>
       </c>
       <c r="X13">
@@ -1461,46 +1633,46 @@
       <c r="E14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="9" t="s">
+      <c r="H14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="P14" s="2" t="s">
-        <v>19</v>
+      <c r="P14" s="18" t="s">
+        <v>21</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="S14" s="5" t="s">
+      <c r="R14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="19" t="s">
         <v>4</v>
       </c>
       <c r="T14" s="5" t="s">
@@ -1532,34 +1704,34 @@
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="N15" s="9" t="s">
+      <c r="G15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="O15" s="2" t="s">
@@ -1571,13 +1743,13 @@
       <c r="Q15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R15" s="5" t="s">
+      <c r="R15" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="T15" s="24" t="s">
         <v>4</v>
       </c>
       <c r="U15" s="5" t="s">
@@ -1621,7 +1793,7 @@
       <c r="I16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="17" t="s">
         <v>19</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -1645,7 +1817,7 @@
       <c r="Q16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R16" s="5" t="s">
+      <c r="R16" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S16" s="5" t="s">
@@ -1707,7 +1879,7 @@
       <c r="M17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="O17" s="2" t="s">
@@ -1719,7 +1891,7 @@
       <c r="Q17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R17" s="5" t="s">
+      <c r="R17" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S17" s="5" t="s">
@@ -1751,7 +1923,7 @@
       <c r="C18" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1778,13 +1950,13 @@
       <c r="L18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="M18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="O18" s="19" t="s">
         <v>7</v>
       </c>
       <c r="P18" s="5" t="s">
@@ -1793,7 +1965,7 @@
       <c r="Q18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R18" s="5" t="s">
+      <c r="R18" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S18" s="5" t="s">
@@ -1822,13 +1994,13 @@
       <c r="B19" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="28" t="s">
         <v>19</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -1855,7 +2027,7 @@
       <c r="M19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="19" t="s">
         <v>7</v>
       </c>
       <c r="O19" s="5" t="s">
@@ -1867,7 +2039,7 @@
       <c r="Q19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="R19" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S19" s="5" t="s">
@@ -1899,7 +2071,7 @@
       <c r="C20" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1911,7 +2083,7 @@
       <c r="G20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H20" s="8" t="s">
+      <c r="H20" s="21" t="s">
         <v>6</v>
       </c>
       <c r="I20" s="5" t="s">
@@ -1941,7 +2113,7 @@
       <c r="Q20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R20" s="5" t="s">
+      <c r="R20" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S20" s="5" t="s">
@@ -1982,13 +2154,13 @@
       <c r="F21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="28" t="s">
         <v>19</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="19" t="s">
         <v>6</v>
       </c>
       <c r="J21" s="5" t="s">
@@ -2015,7 +2187,7 @@
       <c r="Q21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="19" t="s">
         <v>4</v>
       </c>
       <c r="S21" s="5" t="s">
@@ -2030,8 +2202,8 @@
       <c r="V21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="W21" s="5" t="s">
-        <v>4</v>
+      <c r="W21" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="X21">
         <v>20</v>
@@ -2108,7 +2280,648 @@
         <v>22</v>
       </c>
     </row>
+    <row r="25" spans="1:24" ht="31" x14ac:dyDescent="0.35">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="I25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="J25" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q25" s="34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14"/>
+    </row>
+    <row r="27" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:24" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="22"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="11"/>
+      <c r="X30" s="11"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+      <c r="W31" s="11"/>
+      <c r="X31" s="11"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+      <c r="V36" s="11"/>
+      <c r="W36" s="11"/>
+      <c r="X36" s="11"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
+      <c r="U37" s="11"/>
+      <c r="V37" s="11"/>
+      <c r="W37" s="11"/>
+      <c r="X37" s="11"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="11"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="11"/>
+      <c r="N38" s="11"/>
+      <c r="O38" s="11"/>
+      <c r="P38" s="11"/>
+      <c r="Q38" s="11"/>
+      <c r="R38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11"/>
+      <c r="W38" s="11"/>
+      <c r="X38" s="11"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="11"/>
+      <c r="X39" s="11"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
+      <c r="V40" s="11"/>
+      <c r="W40" s="11"/>
+      <c r="X40" s="11"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="T41" s="11"/>
+      <c r="U41" s="11"/>
+      <c r="V41" s="11"/>
+      <c r="W41" s="11"/>
+      <c r="X41" s="11"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
+      <c r="S43" s="11"/>
+      <c r="T43" s="11"/>
+      <c r="U43" s="11"/>
+      <c r="V43" s="11"/>
+      <c r="W43" s="11"/>
+      <c r="X43" s="11"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="11"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="11"/>
+      <c r="U44" s="11"/>
+      <c r="V44" s="11"/>
+      <c r="W44" s="11"/>
+      <c r="X44" s="11"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="11"/>
+      <c r="S45" s="11"/>
+      <c r="T45" s="11"/>
+      <c r="U45" s="11"/>
+      <c r="V45" s="11"/>
+      <c r="W45" s="11"/>
+      <c r="X45" s="11"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="11"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="11"/>
+      <c r="U46" s="11"/>
+      <c r="V46" s="11"/>
+      <c r="W46" s="11"/>
+      <c r="X46" s="11"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
+      <c r="V48" s="11"/>
+      <c r="W48" s="11"/>
+      <c r="X48" s="11"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="Q49" s="11"/>
+      <c r="R49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="T49" s="11"/>
+      <c r="U49" s="11"/>
+      <c r="V49" s="11"/>
+      <c r="W49" s="11"/>
+      <c r="X49" s="11"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="Q50" s="11"/>
+      <c r="R50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="T50" s="11"/>
+      <c r="U50" s="11"/>
+      <c r="V50" s="11"/>
+      <c r="W50" s="11"/>
+      <c r="X50" s="11"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="T51" s="11"/>
+      <c r="U51" s="11"/>
+      <c r="V51" s="11"/>
+      <c r="W51" s="11"/>
+      <c r="X51" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>